<commit_message>
cleaning up file organization
</commit_message>
<xml_diff>
--- a/seeds_UNCONFIRMED.xlsx
+++ b/seeds_UNCONFIRMED.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slane84\OneDrive - The University Of British Columbia\Documents\Dissertation\HabitatRecovery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="14_{78DF7D54-BC48-459E-8CEF-35EB6A6F8511}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{6CC3B690-F33E-40B3-BA82-69E9C58B4339}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703CABDA-266A-49CD-97E8-FDF85370BACD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350" xr2:uid="{0BC6CF4E-DA9C-484F-890A-9C39C5660CEB}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4771" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4771" uniqueCount="169">
   <si>
     <t>season</t>
   </si>
@@ -496,9 +496,6 @@
     <t>5b-5c</t>
   </si>
   <si>
-    <t>forb1</t>
-  </si>
-  <si>
     <t>forb2</t>
   </si>
   <si>
@@ -512,12 +509,6 @@
   </si>
   <si>
     <t>poa sp</t>
-  </si>
-  <si>
-    <t>jubu</t>
-  </si>
-  <si>
-    <t>juncus bufonius</t>
   </si>
   <si>
     <r>
@@ -556,6 +547,18 @@
   </si>
   <si>
     <t>3a, 3c</t>
+  </si>
+  <si>
+    <t>jute</t>
+  </si>
+  <si>
+    <t>juncus tenuis</t>
+  </si>
+  <si>
+    <t>epilobium glaberrimum</t>
+  </si>
+  <si>
+    <t>epgl</t>
   </si>
 </sst>
 </file>
@@ -938,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2E3A75-A2C0-44EE-B7B8-200B09E88641}">
   <dimension ref="A1:I683"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C142" sqref="C142"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2490,7 +2493,7 @@
         <v>13</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
@@ -3065,7 +3068,7 @@
         <v>122</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I73" s="6"/>
     </row>
@@ -4713,10 +4716,10 @@
         <v>1</v>
       </c>
       <c r="G130" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H130" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I130" s="6" t="s">
         <v>36</v>
@@ -5032,10 +5035,10 @@
         <v>1</v>
       </c>
       <c r="G141" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H141" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I141" s="6" t="s">
         <v>36</v>
@@ -5061,10 +5064,10 @@
         <v>1</v>
       </c>
       <c r="G142" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H142" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I142" s="6" t="s">
         <v>36</v>
@@ -5525,10 +5528,10 @@
         <v>1</v>
       </c>
       <c r="G158" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H158" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I158" s="6" t="s">
         <v>36</v>
@@ -5815,10 +5818,10 @@
         <v>1</v>
       </c>
       <c r="G168" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H168" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I168" s="6" t="s">
         <v>36</v>
@@ -5902,10 +5905,10 @@
         <v>1</v>
       </c>
       <c r="G171" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H171" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I171" s="6" t="s">
         <v>36</v>
@@ -6018,10 +6021,10 @@
         <v>2</v>
       </c>
       <c r="G175" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H175" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I175" s="6" t="s">
         <v>36</v>
@@ -6105,10 +6108,10 @@
         <v>1</v>
       </c>
       <c r="G178" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H178" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I178" s="6" t="s">
         <v>36</v>
@@ -6221,10 +6224,10 @@
         <v>3</v>
       </c>
       <c r="G182" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H182" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I182" s="6" t="s">
         <v>36</v>
@@ -6656,10 +6659,10 @@
         <v>1</v>
       </c>
       <c r="G197" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H197" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I197" s="6" t="s">
         <v>36</v>
@@ -6743,10 +6746,10 @@
         <v>1</v>
       </c>
       <c r="G200" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H200" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I200" s="6" t="s">
         <v>36</v>
@@ -7062,10 +7065,10 @@
         <v>1</v>
       </c>
       <c r="G211" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H211" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I211" s="6" t="s">
         <v>36</v>
@@ -7381,10 +7384,10 @@
         <v>2</v>
       </c>
       <c r="G222" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H222" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I222" s="6" t="s">
         <v>36</v>
@@ -7439,10 +7442,10 @@
         <v>1</v>
       </c>
       <c r="G224" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H224" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I224" s="6" t="s">
         <v>36</v>
@@ -7613,10 +7616,10 @@
         <v>3</v>
       </c>
       <c r="G230" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H230" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I230" s="6" t="s">
         <v>36</v>
@@ -9005,10 +9008,10 @@
         <v>1</v>
       </c>
       <c r="G278" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H278" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I278" s="6" t="s">
         <v>87</v>
@@ -9382,10 +9385,10 @@
         <v>3</v>
       </c>
       <c r="G291" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H291" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I291" s="6" t="s">
         <v>84</v>
@@ -9585,10 +9588,10 @@
         <v>1</v>
       </c>
       <c r="G298" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H298" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I298" s="6" t="s">
         <v>84</v>
@@ -9672,10 +9675,10 @@
         <v>1</v>
       </c>
       <c r="G301" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H301" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I301" s="6" t="s">
         <v>84</v>
@@ -9933,10 +9936,10 @@
         <v>1</v>
       </c>
       <c r="G310" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H310" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I310" s="6" t="s">
         <v>84</v>
@@ -10020,10 +10023,10 @@
         <v>2</v>
       </c>
       <c r="G313" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H313" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I313" s="6" t="s">
         <v>84</v>
@@ -10107,10 +10110,10 @@
         <v>1</v>
       </c>
       <c r="G316" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H316" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I316" s="6" t="s">
         <v>84</v>
@@ -10252,10 +10255,10 @@
         <v>3</v>
       </c>
       <c r="G321" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H321" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I321" s="6" t="s">
         <v>84</v>
@@ -10424,10 +10427,10 @@
         <v>2</v>
       </c>
       <c r="G327" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H327" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I327" s="6" t="s">
         <v>84</v>
@@ -10563,16 +10566,16 @@
         <v>3</v>
       </c>
       <c r="E332" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F332" s="4">
         <v>2</v>
       </c>
       <c r="G332" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H332" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I332" s="6" t="s">
         <v>84</v>
@@ -10627,10 +10630,10 @@
         <v>1</v>
       </c>
       <c r="G334" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H334" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I334" s="6" t="s">
         <v>84</v>
@@ -10714,10 +10717,10 @@
         <v>1</v>
       </c>
       <c r="G337" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H337" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I337" s="6" t="s">
         <v>84</v>
@@ -10946,10 +10949,10 @@
         <v>3</v>
       </c>
       <c r="G345" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H345" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I345" s="6" t="s">
         <v>84</v>
@@ -11352,10 +11355,10 @@
         <v>1</v>
       </c>
       <c r="G359" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H359" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I359" s="6" t="s">
         <v>84</v>
@@ -12185,10 +12188,10 @@
         <v>2</v>
       </c>
       <c r="G388" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H388" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I388" s="6" t="s">
         <v>84</v>
@@ -12444,10 +12447,10 @@
         <v>1</v>
       </c>
       <c r="G397" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H397" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I397" s="6" t="s">
         <v>84</v>
@@ -14321,7 +14324,7 @@
         <v>2</v>
       </c>
       <c r="E462" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F462" s="4">
         <v>2</v>
@@ -16117,7 +16120,7 @@
         <v>2</v>
       </c>
       <c r="E524" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F524" s="4">
         <v>4</v>
@@ -16850,7 +16853,7 @@
         <v>18</v>
       </c>
       <c r="I549" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="550" spans="1:9" x14ac:dyDescent="0.35">
@@ -16960,10 +16963,10 @@
         <v>3</v>
       </c>
       <c r="G553" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H553" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I553" s="6" t="s">
         <v>90</v>
@@ -17047,10 +17050,10 @@
         <v>1</v>
       </c>
       <c r="G556" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H556" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I556" s="6" t="s">
         <v>90</v>
@@ -17250,10 +17253,10 @@
         <v>1</v>
       </c>
       <c r="G563" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H563" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I563" s="6" t="s">
         <v>90</v>
@@ -17424,10 +17427,10 @@
         <v>2</v>
       </c>
       <c r="G569" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H569" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I569" s="6" t="s">
         <v>90</v>
@@ -17511,10 +17514,10 @@
         <v>1</v>
       </c>
       <c r="G572" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H572" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I572" s="6" t="s">
         <v>90</v>
@@ -18062,10 +18065,10 @@
         <v>1</v>
       </c>
       <c r="G591" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H591" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I591" s="6" t="s">
         <v>90</v>
@@ -18636,7 +18639,7 @@
         <v>6</v>
       </c>
       <c r="E611" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F611" s="4">
         <v>2</v>
@@ -18671,10 +18674,10 @@
         <v>1</v>
       </c>
       <c r="G612" s="4" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="H612" s="4" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="I612" s="6" t="s">
         <v>93</v>
@@ -18700,10 +18703,10 @@
         <v>1</v>
       </c>
       <c r="G613" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H613" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I613" s="6" t="s">
         <v>90</v>
@@ -18845,10 +18848,10 @@
         <v>2</v>
       </c>
       <c r="G618" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H618" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I618" s="6" t="s">
         <v>90</v>
@@ -18926,16 +18929,16 @@
         <v>8</v>
       </c>
       <c r="E621" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F621" s="4">
         <v>2</v>
       </c>
       <c r="G621" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H621" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I621" s="6" t="s">
         <v>90</v>
@@ -18955,7 +18958,7 @@
         <v>8</v>
       </c>
       <c r="E622" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F622" s="4">
         <v>2</v>
@@ -19512,10 +19515,10 @@
         <v>1</v>
       </c>
       <c r="G641" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H641" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I641" s="6" t="s">
         <v>95</v>
@@ -19921,7 +19924,7 @@
         <v>122</v>
       </c>
       <c r="H655" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I655" s="6" t="s">
         <v>98</v>
@@ -20978,18 +20981,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21012,6 +21015,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2CD57BB-D08A-4DFF-9316-96A2B7916FDF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5149C0F-79C8-4B3B-B7C7-9D5FF5A21D35}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -21026,12 +21037,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2CD57BB-D08A-4DFF-9316-96A2B7916FDF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>